<commit_message>
Fix: ajustes gerais no módulo alimentos (frontend + backend) versão GPT3
</commit_message>
<xml_diff>
--- a/tabelas_mod_alimentos.xlsx
+++ b/tabelas_mod_alimentos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slima\Desktop\fit_plus_v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915E0D65-415A-4C82-8049-2E2D3499BC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBB9AE3-391B-4D32-95FB-AE35C5DD091C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,7 @@
     <sheet name="status_registro" sheetId="6" r:id="rId7"/>
     <sheet name="tipo_registro_alimento" sheetId="7" r:id="rId8"/>
     <sheet name="tipo_medida" sheetId="9" r:id="rId9"/>
+    <sheet name="alergicos" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tbl_alimentos!$A$1:$G$47</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="355">
   <si>
     <t>id</t>
   </si>
@@ -769,9 +770,6 @@
     <t>Contém glúten</t>
   </si>
   <si>
-    <t>Alérgicos Comuns</t>
-  </si>
-  <si>
     <t>Usuário que registrou o item</t>
   </si>
   <si>
@@ -860,6 +858,258 @@
   </si>
   <si>
     <t>tbl_aux_tipo_medida</t>
+  </si>
+  <si>
+    <t>Alergenicos e Intolerancias Comuns</t>
+  </si>
+  <si>
+    <t>tbl_aux_alergicos</t>
+  </si>
+  <si>
+    <t>Leite</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ ProteÃ­nas do leite (caseÃ­na, soro)</t>
+  </si>
+  <si>
+    <t>Ovos</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Clara e gema</t>
+  </si>
+  <si>
+    <t>GlÃºten</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Presente no trigo, cevada e centeio</t>
+  </si>
+  <si>
+    <t>Amendoim</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Forte potencial anafilÃ¡tico</t>
+  </si>
+  <si>
+    <t>Frutos do mar</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Inclui peixes, crustÃ¡ceos e moluscos</t>
+  </si>
+  <si>
+    <t>Soja</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Presente em Ã³leos, molhos, produtos processados</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>2025-07-21 13:22:40.34208</t>
+  </si>
+  <si>
+    <t>Trigo</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Causa alergia ou pode estar ligado Ã  intolerÃ¢ncia ao glÃºten</t>
+  </si>
+  <si>
+    <t>Castanhas (em geral)</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Ex: noz, pecÃ£, castanha-do-parÃ¡</t>
+  </si>
+  <si>
+    <t>Lactose</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ AÃ§Ãºcar do leite</t>
+  </si>
+  <si>
+    <t>Corantes artificiais</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ ReaÃ§Ãµes nÃ£o imunolÃ³gicas</t>
+  </si>
+  <si>
+    <t>Gergelim</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Presente em pÃ£es, biscoitos e condimentos</t>
+  </si>
+  <si>
+    <t>Nozes-macadÃ¢mia</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Presente em doces, bolos, cookies</t>
+  </si>
+  <si>
+    <t>Caju (castanha de caju)</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Alergia frequente no Brasil, especialmente entre crianÃ§as</t>
+  </si>
+  <si>
+    <t>AvelÃ£</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Presente em chocolates e cremes</t>
+  </si>
+  <si>
+    <t>Pistache</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Mais comum em misturas de nuts e sobremesas</t>
+  </si>
+  <si>
+    <t>Milho</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Pode causar reaÃ§Ãµes digestivas em sensÃ­veis</t>
+  </si>
+  <si>
+    <t>AmÃªndoas</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Muito usada em confeitaria, leite vegetal</t>
+  </si>
+  <si>
+    <t>Sementes de girassol</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Presente em barras, pÃ£es e granolas</t>
+  </si>
+  <si>
+    <t>Sulfitos</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Conservante comum</t>
+  </si>
+  <si>
+    <t>Mostarda</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Condimento que causa alergia, mesmo em pequenas quantidades</t>
+  </si>
+  <si>
+    <t>Aditivos alimentares</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ ReaÃ§Ãµes a glutamato monossÃ³dico (MSG), nitratos, entre outros</t>
+  </si>
+  <si>
+    <t>CafÃ© / cafeÃ­na</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Estimula o sistema nervoso</t>
+  </si>
+  <si>
+    <t>Frutose</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ AÃ§Ãºcar natural das frutas</t>
+  </si>
+  <si>
+    <t>AÃ§Ãºcar refinado</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Sensibilidade Ã  absorÃ§Ã£o</t>
+  </si>
+  <si>
+    <t>Chocolate</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ ContÃ©m cafeÃ­na, aÃ§Ãºcar e traÃ§os de leite</t>
+  </si>
+  <si>
+    <t>Tomate</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Possui Ã¡cido e histaminas</t>
+  </si>
+  <si>
+    <t>Canela</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Em sensÃ­veis pode causar urticÃ¡ria ou ardÃªncia bucal</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Pode causar fermentaÃ§Ã£o intestinal ou reaÃ§Ã£o cruzada alÃ©rgica</t>
+  </si>
+  <si>
+    <t>Morango</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Rico em histaminas</t>
+  </si>
+  <si>
+    <t>Alho</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Pode causar inchaÃ§o, gases, refluxo</t>
+  </si>
+  <si>
+    <t>Cebola</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Semelhante ao alho, por compostos sulfurados</t>
+  </si>
+  <si>
+    <t>Pimenta</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Pode causar irritaÃ§Ã£o gÃ¡strica e refluxo</t>
+  </si>
+  <si>
+    <t>Bebidas alcoÃ³licas</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ ReaÃ§Ãµes a Ã¡lcool ou seus componentes (como histaminas, sulfitos)</t>
+  </si>
+  <si>
+    <t>Glutamato monossÃ³dico</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ RealÃ§ador de sabor</t>
+  </si>
+  <si>
+    <t>Bebidas com gÃ¡s</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Podem causar distensÃ£o e gases excessivos</t>
+  </si>
+  <si>
+    <t>Produtos fermentados</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Ex: kefir, kombucha, vinho</t>
+  </si>
+  <si>
+    <t>Oleaginosas</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Grupo geral: amendoim, nozes, castanhas, etc.</t>
+  </si>
+  <si>
+    <t>Lupino</t>
+  </si>
+  <si>
+    <t>AlÃ©rgeno â€“ Farinha de leguminosa</t>
+  </si>
+  <si>
+    <t>ProteÃ­na da carne vermelha</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Pode causar digestÃ£o lenta ou reaÃ§Ãµes a alfa-gal (rara)</t>
+  </si>
+  <si>
+    <t>Histaminas</t>
+  </si>
+  <si>
+    <t>IntolerÃ¢ncia â€“ Presente em queijos, vinho, peixe curado</t>
   </si>
 </sst>
 </file>
@@ -1275,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5126C610-A3B5-4732-B3C4-4FB222671C5D}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,7 +1591,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>170</v>
@@ -1416,7 +1666,7 @@
         <v>37</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>193</v>
@@ -1439,7 +1689,7 @@
         <v>93</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>193</v>
@@ -1453,16 +1703,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>257</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>193</v>
@@ -1531,7 +1781,7 @@
         <v>7</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>190</v>
@@ -1545,10 +1795,10 @@
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="C12" s="3">
         <v>100</v>
@@ -1706,10 +1956,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
@@ -1722,7 +1972,7 @@
         <v>194</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2127,7 +2377,7 @@
         <v>38</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>190</v>
@@ -2150,7 +2400,7 @@
         <v>57</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>190</v>
@@ -2173,7 +2423,7 @@
         <v>71</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>190</v>
@@ -2242,7 +2492,7 @@
         <v>82</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>190</v>
@@ -2256,16 +2506,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>247</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>191</v>
@@ -2274,7 +2524,7 @@
         <v>194</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -2297,7 +2547,7 @@
         <v>194</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>241</v>
+        <v>271</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -2348,13 +2598,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>105</v>
@@ -2363,7 +2613,7 @@
         <v>193</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>198</v>
@@ -2371,6 +2621,770 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G47" xr:uid="{5126C610-A3B5-4732-B3C4-4FB222671C5D}"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7482F42C-D085-4E4E-84B8-F928E5D2E1D5}">
+  <dimension ref="A1:G42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>285</v>
+      </c>
+      <c r="F8" t="s">
+        <v>286</v>
+      </c>
+      <c r="G8" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>285</v>
+      </c>
+      <c r="F9" t="s">
+        <v>286</v>
+      </c>
+      <c r="G9" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>291</v>
+      </c>
+      <c r="C11" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>293</v>
+      </c>
+      <c r="C12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>295</v>
+      </c>
+      <c r="C13" t="s">
+        <v>296</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>285</v>
+      </c>
+      <c r="F13" t="s">
+        <v>286</v>
+      </c>
+      <c r="G13" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>297</v>
+      </c>
+      <c r="C14" t="s">
+        <v>298</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>285</v>
+      </c>
+      <c r="F14" t="s">
+        <v>286</v>
+      </c>
+      <c r="G14" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>299</v>
+      </c>
+      <c r="C15" t="s">
+        <v>300</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>285</v>
+      </c>
+      <c r="F15" t="s">
+        <v>286</v>
+      </c>
+      <c r="G15" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>301</v>
+      </c>
+      <c r="C16" t="s">
+        <v>302</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>285</v>
+      </c>
+      <c r="F16" t="s">
+        <v>286</v>
+      </c>
+      <c r="G16" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>303</v>
+      </c>
+      <c r="C17" t="s">
+        <v>304</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>285</v>
+      </c>
+      <c r="F17" t="s">
+        <v>286</v>
+      </c>
+      <c r="G17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>305</v>
+      </c>
+      <c r="C18" t="s">
+        <v>306</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>285</v>
+      </c>
+      <c r="F18" t="s">
+        <v>286</v>
+      </c>
+      <c r="G18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>307</v>
+      </c>
+      <c r="C19" t="s">
+        <v>308</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" t="s">
+        <v>285</v>
+      </c>
+      <c r="F19" t="s">
+        <v>286</v>
+      </c>
+      <c r="G19" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>309</v>
+      </c>
+      <c r="C20" t="s">
+        <v>310</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>285</v>
+      </c>
+      <c r="F20" t="s">
+        <v>286</v>
+      </c>
+      <c r="G20" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>311</v>
+      </c>
+      <c r="C21" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>313</v>
+      </c>
+      <c r="C22" t="s">
+        <v>314</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>285</v>
+      </c>
+      <c r="F22" t="s">
+        <v>286</v>
+      </c>
+      <c r="G22" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>315</v>
+      </c>
+      <c r="C23" t="s">
+        <v>316</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>285</v>
+      </c>
+      <c r="F23" t="s">
+        <v>286</v>
+      </c>
+      <c r="G23" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>317</v>
+      </c>
+      <c r="C24" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>319</v>
+      </c>
+      <c r="C25" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>321</v>
+      </c>
+      <c r="C26" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>323</v>
+      </c>
+      <c r="C27" t="s">
+        <v>324</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>285</v>
+      </c>
+      <c r="F27" t="s">
+        <v>286</v>
+      </c>
+      <c r="G27" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>325</v>
+      </c>
+      <c r="C28" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>327</v>
+      </c>
+      <c r="C29" t="s">
+        <v>328</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" t="s">
+        <v>285</v>
+      </c>
+      <c r="F29" t="s">
+        <v>286</v>
+      </c>
+      <c r="G29" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>329</v>
+      </c>
+      <c r="C30" t="s">
+        <v>330</v>
+      </c>
+      <c r="D30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" t="s">
+        <v>285</v>
+      </c>
+      <c r="F30" t="s">
+        <v>286</v>
+      </c>
+      <c r="G30" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>331</v>
+      </c>
+      <c r="C31" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>333</v>
+      </c>
+      <c r="C32" t="s">
+        <v>334</v>
+      </c>
+      <c r="D32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" t="s">
+        <v>285</v>
+      </c>
+      <c r="F32" t="s">
+        <v>286</v>
+      </c>
+      <c r="G32" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>335</v>
+      </c>
+      <c r="C33" t="s">
+        <v>336</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" t="s">
+        <v>285</v>
+      </c>
+      <c r="F33" t="s">
+        <v>286</v>
+      </c>
+      <c r="G33" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>337</v>
+      </c>
+      <c r="C34" t="s">
+        <v>338</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" t="s">
+        <v>285</v>
+      </c>
+      <c r="F34" t="s">
+        <v>286</v>
+      </c>
+      <c r="G34" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>339</v>
+      </c>
+      <c r="C35" t="s">
+        <v>340</v>
+      </c>
+      <c r="D35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" t="s">
+        <v>285</v>
+      </c>
+      <c r="F35" t="s">
+        <v>286</v>
+      </c>
+      <c r="G35" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>341</v>
+      </c>
+      <c r="C36" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>343</v>
+      </c>
+      <c r="C37" t="s">
+        <v>344</v>
+      </c>
+      <c r="D37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" t="s">
+        <v>285</v>
+      </c>
+      <c r="F37" t="s">
+        <v>286</v>
+      </c>
+      <c r="G37" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>345</v>
+      </c>
+      <c r="C38" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>347</v>
+      </c>
+      <c r="C39" t="s">
+        <v>348</v>
+      </c>
+      <c r="D39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" t="s">
+        <v>285</v>
+      </c>
+      <c r="F39" t="s">
+        <v>286</v>
+      </c>
+      <c r="G39" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>349</v>
+      </c>
+      <c r="C40" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>351</v>
+      </c>
+      <c r="C41" t="s">
+        <v>352</v>
+      </c>
+      <c r="D41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" t="s">
+        <v>285</v>
+      </c>
+      <c r="F41" t="s">
+        <v>286</v>
+      </c>
+      <c r="G41" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>353</v>
+      </c>
+      <c r="C42" t="s">
+        <v>354</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -2396,7 +3410,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2681,7 +3695,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2896,7 +3910,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3055,7 +4069,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3186,7 +4200,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3237,7 +4251,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C4" t="s">
         <v>85</v>
@@ -3303,7 +4317,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3406,7 +4420,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3479,7 +4493,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G4"/>
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3495,7 +4509,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3532,10 +4546,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D3" t="s">
         <v>37</v>
@@ -3546,10 +4560,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Fix: ajustes gerais no módulo alimentos (frontend + backend) versão form report
</commit_message>
<xml_diff>
--- a/tabelas_mod_alimentos.xlsx
+++ b/tabelas_mod_alimentos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slima\Desktop\fit_plus_v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBB9AE3-391B-4D32-95FB-AE35C5DD091C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364AEC2A-AEA1-4ABE-8615-F9477EEACE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tbl_alimentos" sheetId="8" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="tipo_registro_alimento" sheetId="7" r:id="rId8"/>
     <sheet name="tipo_medida" sheetId="9" r:id="rId9"/>
     <sheet name="alergicos" sheetId="10" r:id="rId10"/>
+    <sheet name="report" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tbl_alimentos!$A$1:$G$47</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="379">
   <si>
     <t>id</t>
   </si>
@@ -1110,6 +1111,78 @@
   </si>
   <si>
     <t>IntolerÃ¢ncia â€“ Presente em queijos, vinho, peixe curado</t>
+  </si>
+  <si>
+    <t>id_alimento</t>
+  </si>
+  <si>
+    <t>user_report</t>
+  </si>
+  <si>
+    <t>dt_report</t>
+  </si>
+  <si>
+    <t>status_report</t>
+  </si>
+  <si>
+    <t>open/closed</t>
+  </si>
+  <si>
+    <t>tbl_report</t>
+  </si>
+  <si>
+    <t>tbl_report_itens</t>
+  </si>
+  <si>
+    <t>id_report</t>
+  </si>
+  <si>
+    <t>id_campo</t>
+  </si>
+  <si>
+    <t>valor_sugerido</t>
+  </si>
+  <si>
+    <t>dt_close</t>
+  </si>
+  <si>
+    <t>dt_reg</t>
+  </si>
+  <si>
+    <t>dt_solve</t>
+  </si>
+  <si>
+    <t>tbl_aux_campos_report</t>
+  </si>
+  <si>
+    <t>Calorias</t>
+  </si>
+  <si>
+    <t>Proteinas</t>
+  </si>
+  <si>
+    <t>Açucares Totais</t>
+  </si>
+  <si>
+    <t>Açucares Adicionados</t>
+  </si>
+  <si>
+    <t>Calcio</t>
+  </si>
+  <si>
+    <t>Vitamina E</t>
+  </si>
+  <si>
+    <t>Ômega 3</t>
+  </si>
+  <si>
+    <t>Alérgenos e Intolerâncias Comuns</t>
+  </si>
+  <si>
+    <t>ativo</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1219,6 +1292,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1525,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5126C610-A3B5-4732-B3C4-4FB222671C5D}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2630,7 +2708,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3389,12 +3467,730 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A80246-09C9-4C4A-822B-B4488990CCB4}">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="10"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>369</v>
+      </c>
+      <c r="C12" t="s">
+        <v>377</v>
+      </c>
+      <c r="D12" t="s">
+        <v>285</v>
+      </c>
+      <c r="E12" t="s">
+        <v>378</v>
+      </c>
+      <c r="F12" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>370</v>
+      </c>
+      <c r="C13" t="s">
+        <v>377</v>
+      </c>
+      <c r="D13" t="s">
+        <v>285</v>
+      </c>
+      <c r="E13" t="s">
+        <v>378</v>
+      </c>
+      <c r="F13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C14" t="s">
+        <v>377</v>
+      </c>
+      <c r="D14" t="s">
+        <v>285</v>
+      </c>
+      <c r="E14" t="s">
+        <v>378</v>
+      </c>
+      <c r="F14" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15" t="s">
+        <v>377</v>
+      </c>
+      <c r="D15" t="s">
+        <v>285</v>
+      </c>
+      <c r="E15" t="s">
+        <v>378</v>
+      </c>
+      <c r="F15" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16" t="s">
+        <v>377</v>
+      </c>
+      <c r="D16" t="s">
+        <v>285</v>
+      </c>
+      <c r="E16" t="s">
+        <v>378</v>
+      </c>
+      <c r="F16" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>209</v>
+      </c>
+      <c r="C17" t="s">
+        <v>377</v>
+      </c>
+      <c r="D17" t="s">
+        <v>285</v>
+      </c>
+      <c r="E17" t="s">
+        <v>378</v>
+      </c>
+      <c r="F17" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>202</v>
+      </c>
+      <c r="C18" t="s">
+        <v>377</v>
+      </c>
+      <c r="D18" t="s">
+        <v>285</v>
+      </c>
+      <c r="E18" t="s">
+        <v>378</v>
+      </c>
+      <c r="F18" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>210</v>
+      </c>
+      <c r="C19" t="s">
+        <v>377</v>
+      </c>
+      <c r="D19" t="s">
+        <v>285</v>
+      </c>
+      <c r="E19" t="s">
+        <v>378</v>
+      </c>
+      <c r="F19" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>371</v>
+      </c>
+      <c r="C20" t="s">
+        <v>377</v>
+      </c>
+      <c r="D20" t="s">
+        <v>285</v>
+      </c>
+      <c r="E20" t="s">
+        <v>378</v>
+      </c>
+      <c r="F20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>372</v>
+      </c>
+      <c r="C21" t="s">
+        <v>377</v>
+      </c>
+      <c r="D21" t="s">
+        <v>285</v>
+      </c>
+      <c r="E21" t="s">
+        <v>378</v>
+      </c>
+      <c r="F21" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>229</v>
+      </c>
+      <c r="C22" t="s">
+        <v>377</v>
+      </c>
+      <c r="D22" t="s">
+        <v>285</v>
+      </c>
+      <c r="E22" t="s">
+        <v>378</v>
+      </c>
+      <c r="F22" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>230</v>
+      </c>
+      <c r="C23" t="s">
+        <v>377</v>
+      </c>
+      <c r="D23" t="s">
+        <v>285</v>
+      </c>
+      <c r="E23" t="s">
+        <v>378</v>
+      </c>
+      <c r="F23" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>211</v>
+      </c>
+      <c r="C24" t="s">
+        <v>377</v>
+      </c>
+      <c r="D24" t="s">
+        <v>285</v>
+      </c>
+      <c r="E24" t="s">
+        <v>378</v>
+      </c>
+      <c r="F24" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>373</v>
+      </c>
+      <c r="C25" t="s">
+        <v>377</v>
+      </c>
+      <c r="D25" t="s">
+        <v>285</v>
+      </c>
+      <c r="E25" t="s">
+        <v>378</v>
+      </c>
+      <c r="F25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>203</v>
+      </c>
+      <c r="C26" t="s">
+        <v>377</v>
+      </c>
+      <c r="D26" t="s">
+        <v>285</v>
+      </c>
+      <c r="E26" t="s">
+        <v>378</v>
+      </c>
+      <c r="F26" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>232</v>
+      </c>
+      <c r="C27" t="s">
+        <v>377</v>
+      </c>
+      <c r="D27" t="s">
+        <v>285</v>
+      </c>
+      <c r="E27" t="s">
+        <v>378</v>
+      </c>
+      <c r="F27" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>233</v>
+      </c>
+      <c r="C28" t="s">
+        <v>377</v>
+      </c>
+      <c r="D28" t="s">
+        <v>285</v>
+      </c>
+      <c r="E28" t="s">
+        <v>378</v>
+      </c>
+      <c r="F28" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>204</v>
+      </c>
+      <c r="C29" t="s">
+        <v>377</v>
+      </c>
+      <c r="D29" t="s">
+        <v>285</v>
+      </c>
+      <c r="E29" t="s">
+        <v>378</v>
+      </c>
+      <c r="F29" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>214</v>
+      </c>
+      <c r="C30" t="s">
+        <v>377</v>
+      </c>
+      <c r="D30" t="s">
+        <v>285</v>
+      </c>
+      <c r="E30" t="s">
+        <v>378</v>
+      </c>
+      <c r="F30" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>215</v>
+      </c>
+      <c r="C31" t="s">
+        <v>377</v>
+      </c>
+      <c r="D31" t="s">
+        <v>285</v>
+      </c>
+      <c r="E31" t="s">
+        <v>378</v>
+      </c>
+      <c r="F31" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
+        <v>213</v>
+      </c>
+      <c r="C32" t="s">
+        <v>377</v>
+      </c>
+      <c r="D32" t="s">
+        <v>285</v>
+      </c>
+      <c r="E32" t="s">
+        <v>378</v>
+      </c>
+      <c r="F32" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>216</v>
+      </c>
+      <c r="C33" t="s">
+        <v>377</v>
+      </c>
+      <c r="D33" t="s">
+        <v>285</v>
+      </c>
+      <c r="E33" t="s">
+        <v>378</v>
+      </c>
+      <c r="F33" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>23</v>
+      </c>
+      <c r="B34" t="s">
+        <v>374</v>
+      </c>
+      <c r="C34" t="s">
+        <v>377</v>
+      </c>
+      <c r="D34" t="s">
+        <v>285</v>
+      </c>
+      <c r="E34" t="s">
+        <v>378</v>
+      </c>
+      <c r="F34" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
+        <v>375</v>
+      </c>
+      <c r="C35" t="s">
+        <v>377</v>
+      </c>
+      <c r="D35" t="s">
+        <v>285</v>
+      </c>
+      <c r="E35" t="s">
+        <v>378</v>
+      </c>
+      <c r="F35" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
+        <v>234</v>
+      </c>
+      <c r="C36" t="s">
+        <v>377</v>
+      </c>
+      <c r="D36" t="s">
+        <v>285</v>
+      </c>
+      <c r="E36" t="s">
+        <v>378</v>
+      </c>
+      <c r="F36" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>26</v>
+      </c>
+      <c r="B37" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37" t="s">
+        <v>377</v>
+      </c>
+      <c r="D37" t="s">
+        <v>285</v>
+      </c>
+      <c r="E37" t="s">
+        <v>378</v>
+      </c>
+      <c r="F37" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>219</v>
+      </c>
+      <c r="C38" t="s">
+        <v>377</v>
+      </c>
+      <c r="D38" t="s">
+        <v>285</v>
+      </c>
+      <c r="E38" t="s">
+        <v>378</v>
+      </c>
+      <c r="F38" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>28</v>
+      </c>
+      <c r="B39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" t="s">
+        <v>377</v>
+      </c>
+      <c r="D39" t="s">
+        <v>285</v>
+      </c>
+      <c r="E39" t="s">
+        <v>378</v>
+      </c>
+      <c r="F39" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>29</v>
+      </c>
+      <c r="B40" t="s">
+        <v>376</v>
+      </c>
+      <c r="C40" t="s">
+        <v>377</v>
+      </c>
+      <c r="D40" t="s">
+        <v>285</v>
+      </c>
+      <c r="E40" t="s">
+        <v>378</v>
+      </c>
+      <c r="F40" t="s">
+        <v>378</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A10:F10"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3679,7 +4475,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4404,7 +5200,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4493,7 +5289,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>